<commit_message>
add tables for annotation, prepare meeting minutes
</commit_message>
<xml_diff>
--- a/titlePilotStudy/data/ENG.xlsx
+++ b/titlePilotStudy/data/ENG.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="362">
   <si>
     <t>Identifier</t>
   </si>
@@ -1054,9 +1054,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Vanity Fair: A Novel without a Hero</t>
@@ -1521,9 +1518,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC90" sqref="AC90"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N91" sqref="N91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1628,37 +1625,37 @@
         <v>340</v>
       </c>
       <c r="AC1" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE1" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI1" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="AF1" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="AI1" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ1" s="10" t="s">
-        <v>357</v>
-      </c>
       <c r="AK1" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="AL1" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AM1" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="57.6" x14ac:dyDescent="0.3">
@@ -1810,7 +1807,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>341</v>
@@ -2286,7 +2283,7 @@
         <v>17</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>341</v>
@@ -2403,7 +2400,7 @@
         <v>31</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>341</v>
@@ -2522,7 +2519,7 @@
         <v>47</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>341</v>
@@ -2627,7 +2624,7 @@
         <v>49</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>50</v>
@@ -2639,7 +2636,7 @@
         <v>47</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>341</v>
@@ -2873,7 +2870,7 @@
         <v>47</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>341</v>
@@ -2980,7 +2977,7 @@
         <v>58</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>59</v>
@@ -3464,7 +3461,7 @@
         <v>47</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>341</v>
@@ -4176,7 +4173,7 @@
         <v>47</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>341</v>
@@ -4295,7 +4292,7 @@
         <v>31</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>341</v>
@@ -5116,7 +5113,7 @@
         <v>47</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>341</v>
@@ -5354,7 +5351,7 @@
         <v>31</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>341</v>
@@ -5459,7 +5456,7 @@
         <v>130</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>131</v>
@@ -5471,7 +5468,7 @@
         <v>31</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>341</v>
@@ -5588,7 +5585,7 @@
         <v>17</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>341</v>
@@ -5812,7 +5809,7 @@
         <v>136</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>95</v>
@@ -5824,7 +5821,7 @@
         <v>47</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>341</v>
@@ -7119,7 +7116,7 @@
         <v>47</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L48" s="12" t="s">
         <v>341</v>
@@ -8067,7 +8064,7 @@
         <v>31</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L56" s="12" t="s">
         <v>341</v>
@@ -8541,7 +8538,7 @@
         <v>17</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L60" s="12" t="s">
         <v>341</v>
@@ -9134,7 +9131,7 @@
         <v>17</v>
       </c>
       <c r="K65" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L65" s="12" t="s">
         <v>341</v>
@@ -9239,7 +9236,7 @@
         <v>238</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>239</v>
@@ -10538,7 +10535,7 @@
         <v>275</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H77" s="7" t="s">
         <v>276</v>
@@ -10891,7 +10888,7 @@
         <v>285</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>229</v>
@@ -11603,7 +11600,7 @@
         <v>302</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>303</v>
@@ -12075,7 +12072,7 @@
         <v>311</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>315</v>
@@ -12323,7 +12320,7 @@
         <v>17</v>
       </c>
       <c r="K92" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L92" s="12" t="s">
         <v>341</v>
@@ -12424,7 +12421,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1">
       <formula1>"m,f,d,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K92 O1:O92 AB2:AM92 X1:Y1 M1:M92 R1:R92 AA1:AA92 S2:Z92 L2:L92 N2:N92 P2:Q92">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:Q92 O1:O92 AB2:AM92 X1:Y1 M1:M92 R1:R92 AA1:AA92 S2:Z92 L2:L92 N2:N92 K1:K92">
       <formula1>"yes,no"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH93:AH1048576 AJ93:AJ1048576 AL93:AL1048576 AD93:AD1048576 AL1 AJ1 AH1 AF1 AD1 AF93:AF1048576">
@@ -12629,52 +12626,52 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct tables, or remove last rows
</commit_message>
<xml_diff>
--- a/titlePilotStudy/data/ENG.xlsx
+++ b/titlePilotStudy/data/ENG.xlsx
@@ -1934,7 +1934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2007,6 +2007,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -7994,15 +8007,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU5" sqref="AU5"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="7" width="10.88671875" customWidth="1"/>
+    <col min="2" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="30" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
     <col min="8" max="8" width="31.109375" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.88671875" style="2" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="10" customWidth="1"/>
@@ -8038,7 +8053,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="26" t="s">
         <v>572</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -8208,7 +8223,7 @@
       <c r="E2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="27">
         <v>1840</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -8371,7 +8386,7 @@
       <c r="E3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="27">
         <v>1841</v>
       </c>
       <c r="G3" s="16" t="s">
@@ -8536,7 +8551,7 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="27">
         <v>1841</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -8701,7 +8716,7 @@
       <c r="E5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="27">
         <v>1844</v>
       </c>
       <c r="G5" s="16" t="s">
@@ -8866,7 +8881,7 @@
       <c r="E6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="27">
         <v>1845</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -9031,7 +9046,7 @@
       <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="27">
         <v>1846</v>
       </c>
       <c r="G7" s="16" t="s">
@@ -9194,7 +9209,7 @@
       <c r="E8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="27">
         <v>1847</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -9359,7 +9374,7 @@
       <c r="E9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="27">
         <v>1847</v>
       </c>
       <c r="G9" s="16" t="s">
@@ -9522,7 +9537,7 @@
       <c r="E10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="27">
         <v>1848</v>
       </c>
       <c r="G10" s="16" t="s">
@@ -9685,7 +9700,7 @@
       <c r="E11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="27">
         <v>1848</v>
       </c>
       <c r="G11" s="16" t="s">
@@ -9848,7 +9863,7 @@
       <c r="E12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="27">
         <v>1848</v>
       </c>
       <c r="G12" s="16" t="s">
@@ -10013,7 +10028,7 @@
       <c r="E13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="27">
         <v>1849</v>
       </c>
       <c r="G13" s="16" t="s">
@@ -10170,7 +10185,7 @@
       <c r="E14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="27">
         <v>1850</v>
       </c>
       <c r="G14" s="16" t="s">
@@ -10333,7 +10348,7 @@
       <c r="E15" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="27">
         <v>1851</v>
       </c>
       <c r="G15" s="16" t="s">
@@ -10498,7 +10513,7 @@
       <c r="E16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="27">
         <v>1851</v>
       </c>
       <c r="G16" s="16" t="s">
@@ -10663,7 +10678,7 @@
       <c r="E17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="27">
         <v>1853</v>
       </c>
       <c r="G17" s="16" t="s">
@@ -10828,7 +10843,7 @@
       <c r="E18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="27">
         <v>1853</v>
       </c>
       <c r="G18" s="16" t="s">
@@ -10991,7 +11006,7 @@
       <c r="E19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="27">
         <v>1854</v>
       </c>
       <c r="G19" s="16" t="s">
@@ -11156,7 +11171,7 @@
       <c r="E20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="27">
         <v>1855</v>
       </c>
       <c r="G20" s="16" t="s">
@@ -11319,7 +11334,7 @@
       <c r="E21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="27">
         <v>1856</v>
       </c>
       <c r="G21" s="16" t="s">
@@ -11484,7 +11499,7 @@
       <c r="E22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="27">
         <v>1856</v>
       </c>
       <c r="G22" s="16" t="s">
@@ -11647,7 +11662,7 @@
       <c r="E23" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="27">
         <v>1857</v>
       </c>
       <c r="G23" s="16" t="s">
@@ -11812,7 +11827,7 @@
       <c r="E24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="27">
         <v>1860</v>
       </c>
       <c r="G24" s="16" t="s">
@@ -11977,7 +11992,7 @@
       <c r="E25" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="28">
         <v>1861</v>
       </c>
       <c r="G25" s="16" t="s">
@@ -12140,7 +12155,7 @@
       <c r="E26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="27">
         <v>1862</v>
       </c>
       <c r="G26" s="16" t="s">
@@ -12303,7 +12318,7 @@
       <c r="E27" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="27">
         <v>1863</v>
       </c>
       <c r="G27" s="16" t="s">
@@ -12466,7 +12481,7 @@
       <c r="E28" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="27">
         <v>1863</v>
       </c>
       <c r="G28" s="16" t="s">
@@ -12631,7 +12646,7 @@
       <c r="E29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="27">
         <v>1863</v>
       </c>
       <c r="G29" s="16" t="s">
@@ -12794,7 +12809,7 @@
       <c r="E30" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="27">
         <v>1864</v>
       </c>
       <c r="G30" s="16" t="s">
@@ -12957,7 +12972,7 @@
       <c r="E31" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="27">
         <v>1864</v>
       </c>
       <c r="G31" s="16" t="s">
@@ -13122,7 +13137,7 @@
       <c r="E32" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="27">
         <v>1865</v>
       </c>
       <c r="G32" s="16" t="s">
@@ -13285,7 +13300,7 @@
       <c r="E33" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="27">
         <v>1865</v>
       </c>
       <c r="G33" s="16" t="s">
@@ -13450,7 +13465,7 @@
       <c r="E34" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="27">
         <v>1866</v>
       </c>
       <c r="G34" s="16" t="s">
@@ -13615,7 +13630,7 @@
       <c r="E35" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="28">
         <v>1867</v>
       </c>
       <c r="G35" s="16" t="s">
@@ -13778,7 +13793,7 @@
       <c r="E36" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="28">
         <v>1870</v>
       </c>
       <c r="G36" s="16" t="s">
@@ -13941,7 +13956,7 @@
       <c r="E37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="28">
         <v>1870</v>
       </c>
       <c r="G37" s="16" t="s">
@@ -14104,7 +14119,7 @@
       <c r="E38" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="28">
         <v>1871</v>
       </c>
       <c r="G38" s="16" t="s">
@@ -14269,7 +14284,7 @@
       <c r="E39" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="27">
         <v>1872</v>
       </c>
       <c r="G39" s="16" t="s">
@@ -14432,7 +14447,7 @@
       <c r="E40" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="27">
         <v>1872</v>
       </c>
       <c r="G40" s="16" t="s">
@@ -14595,7 +14610,7 @@
       <c r="E41" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="28">
         <v>1874</v>
       </c>
       <c r="G41" s="16" t="s">
@@ -14758,7 +14773,7 @@
       <c r="E42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="27">
         <v>1874</v>
       </c>
       <c r="G42" s="16" t="s">
@@ -14921,7 +14936,7 @@
       <c r="E43" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="27">
         <v>1874</v>
       </c>
       <c r="G43" s="16" t="s">
@@ -15084,7 +15099,7 @@
       <c r="E44" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="19">
+      <c r="F44" s="28">
         <v>1876</v>
       </c>
       <c r="G44" s="16" t="s">
@@ -15247,7 +15262,7 @@
       <c r="E45" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="27">
         <v>1877</v>
       </c>
       <c r="G45" s="16" t="s">
@@ -15410,7 +15425,7 @@
       <c r="E46" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="16">
+      <c r="F46" s="27">
         <v>1880</v>
       </c>
       <c r="G46" s="16" t="s">
@@ -15575,7 +15590,7 @@
       <c r="E47" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="19">
+      <c r="F47" s="28">
         <v>1882</v>
       </c>
       <c r="G47" s="16" t="s">
@@ -15740,7 +15755,7 @@
       <c r="E48" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="19">
+      <c r="F48" s="28">
         <v>1883</v>
       </c>
       <c r="G48" s="16" t="s">
@@ -15905,7 +15920,7 @@
       <c r="E49" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="16">
+      <c r="F49" s="27">
         <v>1883</v>
       </c>
       <c r="G49" s="16" t="s">
@@ -16070,7 +16085,7 @@
       <c r="E50" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F50" s="27">
         <v>1884</v>
       </c>
       <c r="G50" s="16" t="s">
@@ -16235,7 +16250,7 @@
       <c r="E51" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="19">
+      <c r="F51" s="28">
         <v>1885</v>
       </c>
       <c r="G51" s="16" t="s">
@@ -16398,7 +16413,7 @@
       <c r="E52" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="19">
+      <c r="F52" s="28">
         <v>1886</v>
       </c>
       <c r="G52" s="16" t="s">
@@ -16563,7 +16578,7 @@
       <c r="E53" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="19">
+      <c r="F53" s="28">
         <v>1887</v>
       </c>
       <c r="G53" s="16" t="s">
@@ -16728,7 +16743,7 @@
       <c r="E54" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="16">
+      <c r="F54" s="27">
         <v>1887</v>
       </c>
       <c r="G54" s="16" t="s">
@@ -16891,7 +16906,7 @@
       <c r="E55" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F55" s="16">
+      <c r="F55" s="27">
         <v>1887</v>
       </c>
       <c r="G55" s="16" t="s">
@@ -17056,7 +17071,7 @@
       <c r="E56" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="16">
+      <c r="F56" s="27">
         <v>1889</v>
       </c>
       <c r="G56" s="16" t="s">
@@ -17221,7 +17236,7 @@
       <c r="E57" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="27">
         <v>1890</v>
       </c>
       <c r="G57" s="16" t="s">
@@ -17384,7 +17399,7 @@
       <c r="E58" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="19">
+      <c r="F58" s="28">
         <v>1890</v>
       </c>
       <c r="G58" s="16" t="s">
@@ -17549,7 +17564,7 @@
       <c r="E59" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F59" s="19">
+      <c r="F59" s="28">
         <v>1891</v>
       </c>
       <c r="G59" s="16" t="s">
@@ -17714,7 +17729,7 @@
       <c r="E60" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="19">
+      <c r="F60" s="28">
         <v>1891</v>
       </c>
       <c r="G60" s="16" t="s">
@@ -17879,7 +17894,7 @@
       <c r="E61" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F61" s="27">
         <v>1892</v>
       </c>
       <c r="G61" s="16" t="s">
@@ -18042,7 +18057,7 @@
       <c r="E62" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F62" s="19">
+      <c r="F62" s="28">
         <v>1893</v>
       </c>
       <c r="G62" s="16" t="s">
@@ -18205,7 +18220,7 @@
       <c r="E63" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="19">
+      <c r="F63" s="28">
         <v>1893</v>
       </c>
       <c r="G63" s="16" t="s">
@@ -18370,7 +18385,7 @@
       <c r="E64" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="16">
+      <c r="F64" s="27">
         <v>1894</v>
       </c>
       <c r="G64" s="16" t="s">
@@ -18535,7 +18550,7 @@
       <c r="E65" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="19">
+      <c r="F65" s="28">
         <v>1894</v>
       </c>
       <c r="G65" s="16" t="s">
@@ -18700,7 +18715,7 @@
       <c r="E66" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F66" s="27">
         <v>1895</v>
       </c>
       <c r="G66" s="16" t="s">
@@ -18865,7 +18880,7 @@
       <c r="E67" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F67" s="16">
+      <c r="F67" s="27">
         <v>1895</v>
       </c>
       <c r="G67" s="16" t="s">
@@ -19030,7 +19045,7 @@
       <c r="E68" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F68" s="19">
+      <c r="F68" s="28">
         <v>1895</v>
       </c>
       <c r="G68" s="16" t="s">
@@ -19193,7 +19208,7 @@
       <c r="E69" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F69" s="16">
+      <c r="F69" s="27">
         <v>1895</v>
       </c>
       <c r="G69" s="16" t="s">
@@ -19356,7 +19371,7 @@
       <c r="E70" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F70" s="16">
+      <c r="F70" s="27">
         <v>1895</v>
       </c>
       <c r="G70" s="16" t="s">
@@ -19521,7 +19536,7 @@
       <c r="E71" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F71" s="16">
+      <c r="F71" s="27">
         <v>1896</v>
       </c>
       <c r="G71" s="16" t="s">
@@ -19684,7 +19699,7 @@
       <c r="E72" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F72" s="16">
+      <c r="F72" s="27">
         <v>1896</v>
       </c>
       <c r="G72" s="16" t="s">
@@ -19847,7 +19862,7 @@
       <c r="E73" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="16">
+      <c r="F73" s="27">
         <v>1897</v>
       </c>
       <c r="G73" s="16" t="s">
@@ -20012,7 +20027,7 @@
       <c r="E74" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F74" s="16">
+      <c r="F74" s="27">
         <v>1897</v>
       </c>
       <c r="G74" s="16" t="s">
@@ -20177,7 +20192,7 @@
       <c r="E75" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F75" s="19">
+      <c r="F75" s="28">
         <v>1897</v>
       </c>
       <c r="G75" s="16" t="s">
@@ -20342,7 +20357,7 @@
       <c r="E76" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F76" s="16">
+      <c r="F76" s="27">
         <v>1898</v>
       </c>
       <c r="G76" s="16" t="s">
@@ -20505,7 +20520,7 @@
       <c r="E77" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F77" s="16">
+      <c r="F77" s="27">
         <v>1900</v>
       </c>
       <c r="G77" s="16" t="s">
@@ -20670,7 +20685,7 @@
       <c r="E78" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="16">
+      <c r="F78" s="27">
         <v>1900</v>
       </c>
       <c r="G78" s="16" t="s">
@@ -20833,7 +20848,7 @@
       <c r="E79" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="19">
+      <c r="F79" s="28">
         <v>1900</v>
       </c>
       <c r="G79" s="16" t="s">
@@ -20996,7 +21011,7 @@
       <c r="E80" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F80" s="16">
+      <c r="F80" s="27">
         <v>1901</v>
       </c>
       <c r="G80" s="16" t="s">
@@ -21161,7 +21176,7 @@
       <c r="E81" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F81" s="16">
+      <c r="F81" s="27">
         <v>1901</v>
       </c>
       <c r="G81" s="16" t="s">
@@ -21326,7 +21341,7 @@
       <c r="E82" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F82" s="16">
+      <c r="F82" s="27">
         <v>1902</v>
       </c>
       <c r="G82" s="16" t="s">
@@ -21489,7 +21504,7 @@
       <c r="E83" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F83" s="16">
+      <c r="F83" s="27">
         <v>1903</v>
       </c>
       <c r="G83" s="16" t="s">
@@ -21654,7 +21669,7 @@
       <c r="E84" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F84" s="16">
+      <c r="F84" s="27">
         <v>1906</v>
       </c>
       <c r="G84" s="16" t="s">
@@ -21819,7 +21834,7 @@
       <c r="E85" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F85" s="16">
+      <c r="F85" s="27">
         <v>1907</v>
       </c>
       <c r="G85" s="16" t="s">
@@ -21984,7 +21999,7 @@
       <c r="E86" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F86" s="16">
+      <c r="F86" s="27">
         <v>1907</v>
       </c>
       <c r="G86" s="16" t="s">
@@ -22147,7 +22162,7 @@
       <c r="E87" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F87" s="19">
+      <c r="F87" s="28">
         <v>1908</v>
       </c>
       <c r="G87" s="16" t="s">
@@ -22310,7 +22325,7 @@
       <c r="E88" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F88" s="16">
+      <c r="F88" s="27">
         <v>1909</v>
       </c>
       <c r="G88" s="16" t="s">
@@ -22475,7 +22490,7 @@
       <c r="E89" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F89" s="19">
+      <c r="F89" s="28">
         <v>1909</v>
       </c>
       <c r="G89" s="16" t="s">
@@ -22640,7 +22655,7 @@
       <c r="E90" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F90" s="21">
+      <c r="F90" s="29">
         <v>1910</v>
       </c>
       <c r="G90" s="16" t="s">
@@ -22805,7 +22820,7 @@
       <c r="E91" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F91" s="16">
+      <c r="F91" s="27">
         <v>1911</v>
       </c>
       <c r="G91" s="16" t="s">
@@ -22970,7 +22985,7 @@
       <c r="E92" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F92" s="16">
+      <c r="F92" s="27">
         <v>1912</v>
       </c>
       <c r="G92" s="16" t="s">
@@ -23135,7 +23150,7 @@
       <c r="E93" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F93" s="16">
+      <c r="F93" s="27">
         <v>1912</v>
       </c>
       <c r="G93" s="16" t="s">
@@ -23299,7 +23314,7 @@
       <c r="E94" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F94" s="16">
+      <c r="F94" s="27">
         <v>1915</v>
       </c>
       <c r="G94" s="16" t="s">
@@ -23463,7 +23478,7 @@
       <c r="E95" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F95" s="16">
+      <c r="F95" s="27">
         <v>1917</v>
       </c>
       <c r="G95" s="16" t="s">
@@ -23627,7 +23642,7 @@
       <c r="E96" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F96" s="16">
+      <c r="F96" s="27">
         <v>1918</v>
       </c>
       <c r="G96" s="16" t="s">
@@ -23791,7 +23806,7 @@
       <c r="E97" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F97" s="16">
+      <c r="F97" s="27">
         <v>1919</v>
       </c>
       <c r="G97" s="16" t="s">
@@ -23953,7 +23968,7 @@
       <c r="E98" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F98" s="16">
+      <c r="F98" s="27">
         <v>1919</v>
       </c>
       <c r="G98" s="16" t="s">
@@ -24115,7 +24130,7 @@
       <c r="E99" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F99" s="16">
+      <c r="F99" s="27">
         <v>1919</v>
       </c>
       <c r="G99" s="16" t="s">
@@ -24277,7 +24292,7 @@
       <c r="E100" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F100" s="16">
+      <c r="F100" s="27">
         <v>1920</v>
       </c>
       <c r="G100" s="16" t="s">
@@ -24441,7 +24456,7 @@
       <c r="E101" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F101" s="16">
+      <c r="F101" s="27">
         <v>1920</v>
       </c>
       <c r="G101" s="16" t="s">

</xml_diff>